<commit_message>
population based on marital status done
</commit_message>
<xml_diff>
--- a/plotly-py-viz-fastapi/datasets/population_marital_data.xlsx
+++ b/plotly-py-viz-fastapi/datasets/population_marital_data.xlsx
@@ -444,24 +444,24 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Toplam</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Erkek</t>
+          <t>erkek</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kadın</t>
+          <t>kadın</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Toplam-Total</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -475,10 +475,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Adana</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>503762</v>
@@ -491,10 +489,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Adıyaman</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>134385</v>
@@ -507,10 +503,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Afyonkarahisar</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>143934</v>
@@ -523,10 +517,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Ağrı</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>125193</v>
@@ -539,10 +531,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Amasya</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>65754</v>
@@ -555,10 +545,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Ankara</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>1337167</v>
@@ -571,10 +559,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Antalya</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>592681</v>
@@ -587,10 +573,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Artvin</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>38629</v>
@@ -603,10 +587,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Aydın</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>227983</v>
@@ -619,10 +601,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Balıkesir</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>233602</v>
@@ -635,10 +615,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Bilecik</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>47826</v>
@@ -651,10 +629,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Bingöl</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>73828</v>
@@ -667,10 +643,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Bitlis</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>89653</v>
@@ -683,10 +657,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Bolu</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>72437</v>
@@ -699,10 +671,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Burdur</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>58793</v>
@@ -715,10 +685,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Bursa</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>648877</v>
@@ -731,10 +699,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Çanakkale</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>116633</v>
@@ -747,10 +713,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Çankırı</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>40023</v>
@@ -763,10 +727,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Çorum</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>95302</v>
@@ -779,10 +741,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Denizli</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>206116</v>
@@ -795,10 +755,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Diyarbakır</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>461909</v>
@@ -811,10 +769,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Edirne</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>90725</v>
@@ -827,10 +783,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Elazığ</t>
-        </is>
+      <c r="A25" s="1" t="n">
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>145753</v>
@@ -843,10 +797,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Erzincan</t>
-        </is>
+      <c r="A26" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>60336</v>
@@ -859,10 +811,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Erzurum</t>
-        </is>
+      <c r="A27" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>187669</v>
@@ -875,10 +825,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>Eskişehir</t>
-        </is>
+      <c r="A28" s="1" t="n">
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>206848</v>
@@ -891,10 +839,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>Gaziantep</t>
-        </is>
+      <c r="A29" s="1" t="n">
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>449834</v>
@@ -907,10 +853,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Giresun</t>
-        </is>
+      <c r="A30" s="1" t="n">
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>96132</v>
@@ -923,10 +867,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Gümüşhane</t>
-        </is>
+      <c r="A31" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>40121</v>
@@ -939,10 +881,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Hakkari</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>97223</v>
@@ -955,10 +895,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>Hatay</t>
-        </is>
+      <c r="A33" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>330180</v>
@@ -971,10 +909,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>Isparta</t>
-        </is>
+      <c r="A34" s="1" t="n">
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>99571</v>
@@ -987,10 +923,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Mersin</t>
-        </is>
+      <c r="A35" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>421986</v>
@@ -1003,10 +937,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>İstanbul</t>
-        </is>
+      <c r="A36" s="1" t="n">
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>4002364</v>
@@ -1019,10 +951,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>İzmir</t>
-        </is>
+      <c r="A37" s="1" t="n">
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>970187</v>
@@ -1035,10 +965,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Kars</t>
-        </is>
+      <c r="A38" s="1" t="n">
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>71250</v>
@@ -1051,10 +979,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Kastamonu</t>
-        </is>
+      <c r="A39" s="1" t="n">
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>75410</v>
@@ -1067,10 +993,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Kayseri</t>
-        </is>
+      <c r="A40" s="1" t="n">
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>300313</v>
@@ -1083,10 +1007,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>Kırklareli</t>
-        </is>
+      <c r="A41" s="1" t="n">
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>78148</v>
@@ -1099,10 +1021,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>Kırşehir</t>
-        </is>
+      <c r="A42" s="1" t="n">
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>53135</v>
@@ -1115,10 +1035,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>Kocaeli</t>
-        </is>
+      <c r="A43" s="1" t="n">
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>447345</v>
@@ -1131,10 +1049,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>Konya</t>
-        </is>
+      <c r="A44" s="1" t="n">
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>473033</v>
@@ -1147,10 +1063,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>Kütahya</t>
-        </is>
+      <c r="A45" s="1" t="n">
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>115517</v>
@@ -1163,10 +1077,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>Malatya</t>
-        </is>
+      <c r="A46" s="1" t="n">
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>173858</v>
@@ -1179,10 +1091,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>Manisa</t>
-        </is>
+      <c r="A47" s="1" t="n">
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>276946</v>
@@ -1195,10 +1105,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>Kahramanmaraş</t>
-        </is>
+      <c r="A48" s="1" t="n">
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>226675</v>
@@ -1211,10 +1119,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>Mardin</t>
-        </is>
+      <c r="A49" s="1" t="n">
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>226824</v>
@@ -1227,10 +1133,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>Muğla</t>
-        </is>
+      <c r="A50" s="1" t="n">
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>220144</v>
@@ -1243,10 +1147,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>Muş</t>
-        </is>
+      <c r="A51" s="1" t="n">
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>100207</v>
@@ -1259,10 +1161,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>Nevşehir</t>
-        </is>
+      <c r="A52" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>63320</v>
@@ -1275,10 +1175,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>Niğde</t>
-        </is>
+      <c r="A53" s="1" t="n">
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>79409</v>
@@ -1291,10 +1189,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>Ordu</t>
-        </is>
+      <c r="A54" s="1" t="n">
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>145058</v>
@@ -1307,10 +1203,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>Rize</t>
-        </is>
+      <c r="A55" s="1" t="n">
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>82222</v>
@@ -1323,10 +1217,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>Sakarya</t>
-        </is>
+      <c r="A56" s="1" t="n">
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>238779</v>
@@ -1339,10 +1231,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>Samsun</t>
-        </is>
+      <c r="A57" s="1" t="n">
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>287046</v>
@@ -1355,10 +1245,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>Siirt</t>
-        </is>
+      <c r="A58" s="1" t="n">
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>95934</v>
@@ -1371,10 +1259,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>Sinop</t>
-        </is>
+      <c r="A59" s="1" t="n">
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>44159</v>
@@ -1387,10 +1273,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>Sivas</t>
-        </is>
+      <c r="A60" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>148422</v>
@@ -1403,10 +1287,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>Tekirdağ</t>
-        </is>
+      <c r="A61" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>231257</v>
@@ -1419,10 +1301,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>Tokat</t>
-        </is>
+      <c r="A62" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>124616</v>
@@ -1435,10 +1315,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>Trabzon</t>
-        </is>
+      <c r="A63" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>189171</v>
@@ -1451,10 +1329,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>Tunceli</t>
-        </is>
+      <c r="A64" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>23740</v>
@@ -1467,10 +1343,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>Şanlıurfa</t>
-        </is>
+      <c r="A65" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="B65" t="n">
         <v>488428</v>
@@ -1483,10 +1357,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>Uşak</t>
-        </is>
+      <c r="A66" s="1" t="n">
+        <v>64</v>
       </c>
       <c r="B66" t="n">
         <v>72638</v>
@@ -1499,10 +1371,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>Van</t>
-        </is>
+      <c r="A67" s="1" t="n">
+        <v>65</v>
       </c>
       <c r="B67" t="n">
         <v>284668</v>
@@ -1515,10 +1385,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>Yozgat</t>
-        </is>
+      <c r="A68" s="1" t="n">
+        <v>66</v>
       </c>
       <c r="B68" t="n">
         <v>87484</v>
@@ -1531,10 +1399,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>Zonguldak</t>
-        </is>
+      <c r="A69" s="1" t="n">
+        <v>67</v>
       </c>
       <c r="B69" t="n">
         <v>126114</v>
@@ -1547,10 +1413,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Aksaray</t>
-        </is>
+      <c r="A70" s="1" t="n">
+        <v>68</v>
       </c>
       <c r="B70" t="n">
         <v>87426</v>
@@ -1563,10 +1427,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>Bayburt</t>
-        </is>
+      <c r="A71" s="1" t="n">
+        <v>69</v>
       </c>
       <c r="B71" t="n">
         <v>24776</v>
@@ -1579,10 +1441,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>Karaman</t>
-        </is>
+      <c r="A72" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="B72" t="n">
         <v>56300</v>
@@ -1595,10 +1455,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>Kırıkkale</t>
-        </is>
+      <c r="A73" s="1" t="n">
+        <v>71</v>
       </c>
       <c r="B73" t="n">
         <v>63379</v>
@@ -1611,10 +1469,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Batman</t>
-        </is>
+      <c r="A74" s="1" t="n">
+        <v>72</v>
       </c>
       <c r="B74" t="n">
         <v>175171</v>
@@ -1627,10 +1483,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>Şırnak</t>
-        </is>
+      <c r="A75" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B75" t="n">
         <v>166693</v>
@@ -1643,10 +1497,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>Bartın</t>
-        </is>
+      <c r="A76" s="1" t="n">
+        <v>74</v>
       </c>
       <c r="B76" t="n">
         <v>43753</v>
@@ -1659,10 +1511,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Ardahan</t>
-        </is>
+      <c r="A77" s="1" t="n">
+        <v>75</v>
       </c>
       <c r="B77" t="n">
         <v>21590</v>
@@ -1675,10 +1525,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Iğdır</t>
-        </is>
+      <c r="A78" s="1" t="n">
+        <v>76</v>
       </c>
       <c r="B78" t="n">
         <v>53746</v>
@@ -1691,10 +1539,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>Yalova</t>
-        </is>
+      <c r="A79" s="1" t="n">
+        <v>77</v>
       </c>
       <c r="B79" t="n">
         <v>68576</v>
@@ -1707,10 +1553,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Karabük</t>
-        </is>
+      <c r="A80" s="1" t="n">
+        <v>78</v>
       </c>
       <c r="B80" t="n">
         <v>66147</v>
@@ -1723,10 +1567,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>Kilis</t>
-        </is>
+      <c r="A81" s="1" t="n">
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>34456</v>
@@ -1739,10 +1581,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Osmaniye</t>
-        </is>
+      <c r="A82" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="B82" t="n">
         <v>117420</v>
@@ -1755,10 +1595,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Düzce</t>
-        </is>
+      <c r="A83" s="1" t="n">
+        <v>81</v>
       </c>
       <c r="B83" t="n">
         <v>87679</v>
@@ -1797,24 +1635,24 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Toplam</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Erkek</t>
+          <t>erkek</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kadın</t>
+          <t>kadın</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Toplam-Total</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1828,10 +1666,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Adana</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>1045322</v>
@@ -1844,10 +1680,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Adıyaman</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>274998</v>
@@ -1860,10 +1694,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Afyonkarahisar</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>388885</v>
@@ -1876,10 +1708,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Ağrı</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>204261</v>
@@ -1892,10 +1722,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Amasya</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>181740</v>
@@ -1908,10 +1736,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Ankara</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>2837059</v>
@@ -1924,10 +1750,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Antalya</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>1313092</v>
@@ -1940,10 +1764,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Artvin</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>90451</v>
@@ -1956,10 +1778,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Aydın</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>592298</v>
@@ -1972,10 +1792,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Balıkesir</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>684640</v>
@@ -1988,10 +1806,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Bilecik</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>117850</v>
@@ -2004,10 +1820,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Bingöl</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>127290</v>
@@ -2020,10 +1834,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Bitlis</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>148583</v>
@@ -2036,10 +1848,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Bolu</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>168618</v>
@@ -2052,10 +1862,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Burdur</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>146243</v>
@@ -2068,10 +1876,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Bursa</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>1633937</v>
@@ -2084,10 +1890,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Çanakkale</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>301774</v>
@@ -2100,10 +1904,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Çankırı</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>112123</v>
@@ -2116,10 +1918,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Çorum</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>286776</v>
@@ -2132,10 +1932,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Denizli</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>548494</v>
@@ -2148,10 +1946,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Diyarbakır</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>725654</v>
@@ -2164,10 +1960,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Edirne</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>220050</v>
@@ -2180,10 +1974,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Elazığ</t>
-        </is>
+      <c r="A25" s="1" t="n">
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>288822</v>
@@ -2196,10 +1988,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Erzincan</t>
-        </is>
+      <c r="A26" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>118493</v>
@@ -2212,10 +2002,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Erzurum</t>
-        </is>
+      <c r="A27" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>339161</v>
@@ -2228,10 +2016,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>Eskişehir</t>
-        </is>
+      <c r="A28" s="1" t="n">
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>454883</v>
@@ -2244,10 +2030,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>Gaziantep</t>
-        </is>
+      <c r="A29" s="1" t="n">
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>951392</v>
@@ -2260,10 +2044,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Giresun</t>
-        </is>
+      <c r="A30" s="1" t="n">
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>244407</v>
@@ -2276,10 +2058,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Gümüşhane</t>
-        </is>
+      <c r="A31" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>73076</v>
@@ -2292,10 +2072,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Hakkari</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>107670</v>
@@ -2308,10 +2086,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>Hatay</t>
-        </is>
+      <c r="A33" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>715248</v>
@@ -2324,10 +2100,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>Isparta</t>
-        </is>
+      <c r="A34" s="1" t="n">
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>230987</v>
@@ -2340,10 +2114,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Mersin</t>
-        </is>
+      <c r="A35" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>921586</v>
@@ -2356,10 +2128,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>İstanbul</t>
-        </is>
+      <c r="A36" s="1" t="n">
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>7263025</v>
@@ -2372,10 +2142,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>İzmir</t>
-        </is>
+      <c r="A37" s="1" t="n">
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>2207233</v>
@@ -2388,10 +2156,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Kars</t>
-        </is>
+      <c r="A38" s="1" t="n">
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>124392</v>
@@ -2404,10 +2170,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Kastamonu</t>
-        </is>
+      <c r="A39" s="1" t="n">
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>212568</v>
@@ -2420,10 +2184,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Kayseri</t>
-        </is>
+      <c r="A40" s="1" t="n">
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>715719</v>
@@ -2436,10 +2198,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>Kırklareli</t>
-        </is>
+      <c r="A41" s="1" t="n">
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>199214</v>
@@ -2452,10 +2212,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>Kırşehir</t>
-        </is>
+      <c r="A42" s="1" t="n">
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>125639</v>
@@ -2468,10 +2226,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>Kocaeli</t>
-        </is>
+      <c r="A43" s="1" t="n">
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>1037635</v>
@@ -2484,10 +2240,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>Konya</t>
-        </is>
+      <c r="A44" s="1" t="n">
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>1153931</v>
@@ -2500,10 +2254,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>Kütahya</t>
-        </is>
+      <c r="A45" s="1" t="n">
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>309460</v>
@@ -2516,10 +2268,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>Malatya</t>
-        </is>
+      <c r="A46" s="1" t="n">
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>360095</v>
@@ -2532,10 +2282,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>Manisa</t>
-        </is>
+      <c r="A47" s="1" t="n">
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>773479</v>
@@ -2548,10 +2296,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>Kahramanmaraş</t>
-        </is>
+      <c r="A48" s="1" t="n">
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>538828</v>
@@ -2564,10 +2310,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>Mardin</t>
-        </is>
+      <c r="A49" s="1" t="n">
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>347838</v>
@@ -2580,10 +2324,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>Muğla</t>
-        </is>
+      <c r="A50" s="1" t="n">
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>547215</v>
@@ -2596,10 +2338,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>Muş</t>
-        </is>
+      <c r="A51" s="1" t="n">
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>160109</v>
@@ -2612,10 +2352,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>Nevşehir</t>
-        </is>
+      <c r="A52" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>162264</v>
@@ -2628,10 +2366,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>Niğde</t>
-        </is>
+      <c r="A53" s="1" t="n">
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>185869</v>
@@ -2644,10 +2380,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>Ordu</t>
-        </is>
+      <c r="A54" s="1" t="n">
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>421237</v>
@@ -2660,10 +2394,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>Rize</t>
-        </is>
+      <c r="A55" s="1" t="n">
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>176014</v>
@@ -2676,10 +2408,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>Sakarya</t>
-        </is>
+      <c r="A56" s="1" t="n">
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>545531</v>
@@ -2692,10 +2422,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>Samsun</t>
-        </is>
+      <c r="A57" s="1" t="n">
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>708392</v>
@@ -2708,10 +2436,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>Siirt</t>
-        </is>
+      <c r="A58" s="1" t="n">
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>134008</v>
@@ -2724,10 +2450,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>Sinop</t>
-        </is>
+      <c r="A59" s="1" t="n">
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>124109</v>
@@ -2740,10 +2464,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>Sivas</t>
-        </is>
+      <c r="A60" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>324649</v>
@@ -2756,10 +2478,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>Tekirdağ</t>
-        </is>
+      <c r="A61" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>597713</v>
@@ -2772,10 +2492,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>Tokat</t>
-        </is>
+      <c r="A62" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>317245</v>
@@ -2788,10 +2506,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>Trabzon</t>
-        </is>
+      <c r="A63" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>416155</v>
@@ -2804,10 +2520,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>Tunceli</t>
-        </is>
+      <c r="A64" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>43503</v>
@@ -2820,10 +2534,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>Şanlıurfa</t>
-        </is>
+      <c r="A65" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="B65" t="n">
         <v>821396</v>
@@ -2836,10 +2548,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>Uşak</t>
-        </is>
+      <c r="A66" s="1" t="n">
+        <v>64</v>
       </c>
       <c r="B66" t="n">
         <v>199469</v>
@@ -2852,10 +2562,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>Van</t>
-        </is>
+      <c r="A67" s="1" t="n">
+        <v>65</v>
       </c>
       <c r="B67" t="n">
         <v>457630</v>
@@ -2868,10 +2576,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>Yozgat</t>
-        </is>
+      <c r="A68" s="1" t="n">
+        <v>66</v>
       </c>
       <c r="B68" t="n">
         <v>218085</v>
@@ -2884,10 +2590,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>Zonguldak</t>
-        </is>
+      <c r="A69" s="1" t="n">
+        <v>67</v>
       </c>
       <c r="B69" t="n">
         <v>311093</v>
@@ -2900,10 +2604,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Aksaray</t>
-        </is>
+      <c r="A70" s="1" t="n">
+        <v>68</v>
       </c>
       <c r="B70" t="n">
         <v>215596</v>
@@ -2916,10 +2618,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>Bayburt</t>
-        </is>
+      <c r="A71" s="1" t="n">
+        <v>69</v>
       </c>
       <c r="B71" t="n">
         <v>40020</v>
@@ -2932,10 +2632,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>Karaman</t>
-        </is>
+      <c r="A72" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="B72" t="n">
         <v>130807</v>
@@ -2948,10 +2646,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>Kırıkkale</t>
-        </is>
+      <c r="A73" s="1" t="n">
+        <v>71</v>
       </c>
       <c r="B73" t="n">
         <v>144422</v>
@@ -2964,10 +2660,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Batman</t>
-        </is>
+      <c r="A74" s="1" t="n">
+        <v>72</v>
       </c>
       <c r="B74" t="n">
         <v>249410</v>
@@ -2980,10 +2674,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>Şırnak</t>
-        </is>
+      <c r="A75" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B75" t="n">
         <v>198220</v>
@@ -2996,10 +2688,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>Bartın</t>
-        </is>
+      <c r="A76" s="1" t="n">
+        <v>74</v>
       </c>
       <c r="B76" t="n">
         <v>110976</v>
@@ -3012,10 +2702,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Ardahan</t>
-        </is>
+      <c r="A77" s="1" t="n">
+        <v>75</v>
       </c>
       <c r="B77" t="n">
         <v>46143</v>
@@ -3028,10 +2716,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Iğdır</t>
-        </is>
+      <c r="A78" s="1" t="n">
+        <v>76</v>
       </c>
       <c r="B78" t="n">
         <v>88648</v>
@@ -3044,10 +2730,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>Yalova</t>
-        </is>
+      <c r="A79" s="1" t="n">
+        <v>77</v>
       </c>
       <c r="B79" t="n">
         <v>148013</v>
@@ -3060,10 +2744,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Karabük</t>
-        </is>
+      <c r="A80" s="1" t="n">
+        <v>78</v>
       </c>
       <c r="B80" t="n">
         <v>126054</v>
@@ -3076,10 +2758,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>Kilis</t>
-        </is>
+      <c r="A81" s="1" t="n">
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>69536</v>
@@ -3092,10 +2772,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Osmaniye</t>
-        </is>
+      <c r="A82" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="B82" t="n">
         <v>266383</v>
@@ -3108,10 +2786,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Düzce</t>
-        </is>
+      <c r="A83" s="1" t="n">
+        <v>81</v>
       </c>
       <c r="B83" t="n">
         <v>205622</v>
@@ -3150,24 +2826,24 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Toplam</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Erkek</t>
+          <t>erkek</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kadın</t>
+          <t>kadın</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Toplam-Total</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -3181,10 +2857,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Adana</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>97420</v>
@@ -3197,10 +2871,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Adıyaman</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>9370</v>
@@ -3213,10 +2885,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Afyonkarahisar</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>22994</v>
@@ -3229,10 +2899,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Ağrı</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>4157</v>
@@ -3245,10 +2913,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Amasya</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>10542</v>
@@ -3261,10 +2927,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Ankara</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>280714</v>
@@ -3277,10 +2941,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Antalya</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>154227</v>
@@ -3293,10 +2955,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Artvin</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>4445</v>
@@ -3309,10 +2969,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Aydın</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>62518</v>
@@ -3325,10 +2983,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Balıkesir</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>63794</v>
@@ -3341,10 +2997,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Bilecik</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>7737</v>
@@ -3357,10 +3011,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Bingöl</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>3248</v>
@@ -3373,10 +3025,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Bitlis</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>2359</v>
@@ -3389,10 +3039,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Bolu</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>11297</v>
@@ -3405,10 +3053,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Burdur</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>10031</v>
@@ -3421,10 +3067,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Bursa</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>123467</v>
@@ -3437,10 +3081,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Çanakkale</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>26546</v>
@@ -3453,10 +3095,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Çankırı</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>5587</v>
@@ -3469,10 +3109,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Çorum</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>17562</v>
@@ -3485,10 +3123,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Denizli</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>49854</v>
@@ -3501,10 +3137,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Diyarbakır</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>21818</v>
@@ -3517,10 +3151,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Edirne</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>18219</v>
@@ -3533,10 +3165,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Elazığ</t>
-        </is>
+      <c r="A25" s="1" t="n">
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>15696</v>
@@ -3549,10 +3179,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Erzincan</t>
-        </is>
+      <c r="A26" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>7225</v>
@@ -3565,10 +3193,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Erzurum</t>
-        </is>
+      <c r="A27" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>11120</v>
@@ -3581,10 +3207,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>Eskişehir</t>
-        </is>
+      <c r="A28" s="1" t="n">
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>45995</v>
@@ -3597,10 +3221,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>Gaziantep</t>
-        </is>
+      <c r="A29" s="1" t="n">
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>50520</v>
@@ -3613,10 +3235,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Giresun</t>
-        </is>
+      <c r="A30" s="1" t="n">
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>16539</v>
@@ -3629,10 +3249,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Gümüşhane</t>
-        </is>
+      <c r="A31" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>3091</v>
@@ -3645,10 +3263,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Hakkari</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>1503</v>
@@ -3661,10 +3277,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>Hatay</t>
-        </is>
+      <c r="A33" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>42698</v>
@@ -3677,10 +3291,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>Isparta</t>
-        </is>
+      <c r="A34" s="1" t="n">
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>15627</v>
@@ -3693,10 +3305,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Mersin</t>
-        </is>
+      <c r="A35" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>89491</v>
@@ -3709,10 +3319,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>İstanbul</t>
-        </is>
+      <c r="A36" s="1" t="n">
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>705408</v>
@@ -3725,10 +3333,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>İzmir</t>
-        </is>
+      <c r="A37" s="1" t="n">
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>290876</v>
@@ -3741,10 +3347,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Kars</t>
-        </is>
+      <c r="A38" s="1" t="n">
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>3882</v>
@@ -3757,10 +3361,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Kastamonu</t>
-        </is>
+      <c r="A39" s="1" t="n">
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>12292</v>
@@ -3773,10 +3375,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Kayseri</t>
-        </is>
+      <c r="A40" s="1" t="n">
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>48240</v>
@@ -3789,10 +3389,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>Kırklareli</t>
-        </is>
+      <c r="A41" s="1" t="n">
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>16983</v>
@@ -3805,10 +3403,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>Kırşehir</t>
-        </is>
+      <c r="A42" s="1" t="n">
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>8781</v>
@@ -3821,10 +3417,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>Kocaeli</t>
-        </is>
+      <c r="A43" s="1" t="n">
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>75459</v>
@@ -3837,10 +3431,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>Konya</t>
-        </is>
+      <c r="A44" s="1" t="n">
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>71861</v>
@@ -3853,10 +3445,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>Kütahya</t>
-        </is>
+      <c r="A45" s="1" t="n">
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>18512</v>
@@ -3869,10 +3459,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>Malatya</t>
-        </is>
+      <c r="A46" s="1" t="n">
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>19846</v>
@@ -3885,10 +3473,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>Manisa</t>
-        </is>
+      <c r="A47" s="1" t="n">
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>55639</v>
@@ -3901,10 +3487,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>Kahramanmaraş</t>
-        </is>
+      <c r="A48" s="1" t="n">
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>27326</v>
@@ -3917,10 +3501,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>Mardin</t>
-        </is>
+      <c r="A49" s="1" t="n">
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>8286</v>
@@ -3933,10 +3515,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>Muğla</t>
-        </is>
+      <c r="A50" s="1" t="n">
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>69039</v>
@@ -3949,10 +3529,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>Muş</t>
-        </is>
+      <c r="A51" s="1" t="n">
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>2472</v>
@@ -3965,10 +3543,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>Nevşehir</t>
-        </is>
+      <c r="A52" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>11737</v>
@@ -3981,10 +3557,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>Niğde</t>
-        </is>
+      <c r="A53" s="1" t="n">
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>11639</v>
@@ -3997,10 +3571,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>Ordu</t>
-        </is>
+      <c r="A54" s="1" t="n">
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>23469</v>
@@ -4013,10 +3585,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>Rize</t>
-        </is>
+      <c r="A55" s="1" t="n">
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>9030</v>
@@ -4029,10 +3599,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>Sakarya</t>
-        </is>
+      <c r="A56" s="1" t="n">
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>38502</v>
@@ -4045,10 +3613,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>Samsun</t>
-        </is>
+      <c r="A57" s="1" t="n">
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>48486</v>
@@ -4061,10 +3627,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>Siirt</t>
-        </is>
+      <c r="A58" s="1" t="n">
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>2239</v>
@@ -4077,10 +3641,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>Sinop</t>
-        </is>
+      <c r="A59" s="1" t="n">
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>8416</v>
@@ -4093,10 +3655,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>Sivas</t>
-        </is>
+      <c r="A60" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>17377</v>
@@ -4109,10 +3669,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>Tekirdağ</t>
-        </is>
+      <c r="A61" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>48086</v>
@@ -4125,10 +3683,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>Tokat</t>
-        </is>
+      <c r="A62" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>16738</v>
@@ -4141,10 +3697,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>Trabzon</t>
-        </is>
+      <c r="A63" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>20138</v>
@@ -4157,10 +3711,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>Tunceli</t>
-        </is>
+      <c r="A64" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>4348</v>
@@ -4173,10 +3725,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>Şanlıurfa</t>
-        </is>
+      <c r="A65" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="B65" t="n">
         <v>21720</v>
@@ -4189,10 +3739,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>Uşak</t>
-        </is>
+      <c r="A66" s="1" t="n">
+        <v>64</v>
       </c>
       <c r="B66" t="n">
         <v>17495</v>
@@ -4205,10 +3753,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>Van</t>
-        </is>
+      <c r="A67" s="1" t="n">
+        <v>65</v>
       </c>
       <c r="B67" t="n">
         <v>8457</v>
@@ -4221,10 +3767,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>Yozgat</t>
-        </is>
+      <c r="A68" s="1" t="n">
+        <v>66</v>
       </c>
       <c r="B68" t="n">
         <v>12096</v>
@@ -4237,10 +3781,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>Zonguldak</t>
-        </is>
+      <c r="A69" s="1" t="n">
+        <v>67</v>
       </c>
       <c r="B69" t="n">
         <v>24725</v>
@@ -4253,10 +3795,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Aksaray</t>
-        </is>
+      <c r="A70" s="1" t="n">
+        <v>68</v>
       </c>
       <c r="B70" t="n">
         <v>15185</v>
@@ -4269,10 +3809,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>Bayburt</t>
-        </is>
+      <c r="A71" s="1" t="n">
+        <v>69</v>
       </c>
       <c r="B71" t="n">
         <v>1344</v>
@@ -4285,10 +3823,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>Karaman</t>
-        </is>
+      <c r="A72" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="B72" t="n">
         <v>10017</v>
@@ -4301,10 +3837,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>Kırıkkale</t>
-        </is>
+      <c r="A73" s="1" t="n">
+        <v>71</v>
       </c>
       <c r="B73" t="n">
         <v>11708</v>
@@ -4317,10 +3851,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Batman</t>
-        </is>
+      <c r="A74" s="1" t="n">
+        <v>72</v>
       </c>
       <c r="B74" t="n">
         <v>5566</v>
@@ -4333,10 +3865,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>Şırnak</t>
-        </is>
+      <c r="A75" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B75" t="n">
         <v>3372</v>
@@ -4349,10 +3879,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>Bartın</t>
-        </is>
+      <c r="A76" s="1" t="n">
+        <v>74</v>
       </c>
       <c r="B76" t="n">
         <v>7636</v>
@@ -4365,10 +3893,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Ardahan</t>
-        </is>
+      <c r="A77" s="1" t="n">
+        <v>75</v>
       </c>
       <c r="B77" t="n">
         <v>1738</v>
@@ -4381,10 +3907,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Iğdır</t>
-        </is>
+      <c r="A78" s="1" t="n">
+        <v>76</v>
       </c>
       <c r="B78" t="n">
         <v>4478</v>
@@ -4397,10 +3921,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>Yalova</t>
-        </is>
+      <c r="A79" s="1" t="n">
+        <v>77</v>
       </c>
       <c r="B79" t="n">
         <v>15368</v>
@@ -4413,10 +3935,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Karabük</t>
-        </is>
+      <c r="A80" s="1" t="n">
+        <v>78</v>
       </c>
       <c r="B80" t="n">
         <v>9069</v>
@@ -4429,10 +3949,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>Kilis</t>
-        </is>
+      <c r="A81" s="1" t="n">
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>3152</v>
@@ -4445,10 +3963,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Osmaniye</t>
-        </is>
+      <c r="A82" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="B82" t="n">
         <v>14624</v>
@@ -4461,10 +3977,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Düzce</t>
-        </is>
+      <c r="A83" s="1" t="n">
+        <v>81</v>
       </c>
       <c r="B83" t="n">
         <v>14944</v>
@@ -4503,24 +4017,24 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Toplam</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Erkek</t>
+          <t>erkek</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kadın</t>
+          <t>kadın</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Toplam-Total</t>
+          <t>toplam</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -4534,10 +4048,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Adana</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>96686</v>
@@ -4550,10 +4062,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Adıyaman</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>21460</v>
@@ -4566,10 +4076,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Afyonkarahisar</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="n">
         <v>42126</v>
@@ -4582,10 +4090,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Ağrı</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="n">
         <v>14127</v>
@@ -4598,10 +4104,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Amasya</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="n">
         <v>22948</v>
@@ -4614,10 +4118,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Ankara</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="n">
         <v>238654</v>
@@ -4630,10 +4132,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Antalya</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B9" t="n">
         <v>99717</v>
@@ -4646,10 +4146,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Artvin</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="n">
         <v>12537</v>
@@ -4662,10 +4160,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Aydın</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="n">
         <v>69993</v>
@@ -4678,10 +4174,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Balıkesir</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="n">
         <v>89517</v>
@@ -4694,10 +4188,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Bilecik</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" t="n">
         <v>13189</v>
@@ -4710,10 +4202,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Bingöl</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B14" t="n">
         <v>9970</v>
@@ -4726,10 +4216,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Bitlis</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B15" t="n">
         <v>9853</v>
@@ -4742,10 +4230,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Bolu</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B16" t="n">
         <v>18883</v>
@@ -4758,10 +4244,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Burdur</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B17" t="n">
         <v>18020</v>
@@ -4774,10 +4258,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Bursa</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="B18" t="n">
         <v>152507</v>
@@ -4790,10 +4272,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Çanakkale</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="B19" t="n">
         <v>38871</v>
@@ -4806,10 +4286,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Çankırı</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B20" t="n">
         <v>13673</v>
@@ -4822,10 +4300,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Çorum</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="B21" t="n">
         <v>35468</v>
@@ -4838,10 +4314,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Denizli</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B22" t="n">
         <v>56869</v>
@@ -4854,10 +4328,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Diyarbakır</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>21</v>
       </c>
       <c r="B23" t="n">
         <v>45419</v>
@@ -4870,10 +4342,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Edirne</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="B24" t="n">
         <v>30447</v>
@@ -4886,10 +4356,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Elazığ</t>
-        </is>
+      <c r="A25" s="1" t="n">
+        <v>23</v>
       </c>
       <c r="B25" t="n">
         <v>28534</v>
@@ -4902,10 +4370,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Erzincan</t>
-        </is>
+      <c r="A26" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="B26" t="n">
         <v>13387</v>
@@ -4918,10 +4384,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Erzurum</t>
-        </is>
+      <c r="A27" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="B27" t="n">
         <v>34153</v>
@@ -4934,10 +4398,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>Eskişehir</t>
-        </is>
+      <c r="A28" s="1" t="n">
+        <v>26</v>
       </c>
       <c r="B28" t="n">
         <v>51998</v>
@@ -4950,10 +4412,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>Gaziantep</t>
-        </is>
+      <c r="A29" s="1" t="n">
+        <v>27</v>
       </c>
       <c r="B29" t="n">
         <v>62250</v>
@@ -4966,10 +4426,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Giresun</t>
-        </is>
+      <c r="A30" s="1" t="n">
+        <v>28</v>
       </c>
       <c r="B30" t="n">
         <v>34099</v>
@@ -4982,10 +4440,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Gümüşhane</t>
-        </is>
+      <c r="A31" s="1" t="n">
+        <v>29</v>
       </c>
       <c r="B31" t="n">
         <v>8354</v>
@@ -4998,10 +4454,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Hakkari</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="B32" t="n">
         <v>5820</v>
@@ -5014,10 +4468,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>Hatay</t>
-        </is>
+      <c r="A33" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="B33" t="n">
         <v>60636</v>
@@ -5030,10 +4482,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>Isparta</t>
-        </is>
+      <c r="A34" s="1" t="n">
+        <v>32</v>
       </c>
       <c r="B34" t="n">
         <v>25498</v>
@@ -5046,10 +4496,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Mersin</t>
-        </is>
+      <c r="A35" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="B35" t="n">
         <v>83480</v>
@@ -5062,10 +4510,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>İstanbul</t>
-        </is>
+      <c r="A36" s="1" t="n">
+        <v>34</v>
       </c>
       <c r="B36" t="n">
         <v>553953</v>
@@ -5078,10 +4524,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>İzmir</t>
-        </is>
+      <c r="A37" s="1" t="n">
+        <v>35</v>
       </c>
       <c r="B37" t="n">
         <v>233437</v>
@@ -5094,10 +4538,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Kars</t>
-        </is>
+      <c r="A38" s="1" t="n">
+        <v>36</v>
       </c>
       <c r="B38" t="n">
         <v>11494</v>
@@ -5110,10 +4552,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Kastamonu</t>
-        </is>
+      <c r="A39" s="1" t="n">
+        <v>37</v>
       </c>
       <c r="B39" t="n">
         <v>30679</v>
@@ -5126,10 +4566,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Kayseri</t>
-        </is>
+      <c r="A40" s="1" t="n">
+        <v>38</v>
       </c>
       <c r="B40" t="n">
         <v>63357</v>
@@ -5142,10 +4580,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>Kırklareli</t>
-        </is>
+      <c r="A41" s="1" t="n">
+        <v>39</v>
       </c>
       <c r="B41" t="n">
         <v>25761</v>
@@ -5158,10 +4594,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>Kırşehir</t>
-        </is>
+      <c r="A42" s="1" t="n">
+        <v>40</v>
       </c>
       <c r="B42" t="n">
         <v>14290</v>
@@ -5174,10 +4608,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>Kocaeli</t>
-        </is>
+      <c r="A43" s="1" t="n">
+        <v>41</v>
       </c>
       <c r="B43" t="n">
         <v>80393</v>
@@ -5190,10 +4622,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>Konya</t>
-        </is>
+      <c r="A44" s="1" t="n">
+        <v>42</v>
       </c>
       <c r="B44" t="n">
         <v>102803</v>
@@ -5206,10 +4636,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>Kütahya</t>
-        </is>
+      <c r="A45" s="1" t="n">
+        <v>43</v>
       </c>
       <c r="B45" t="n">
         <v>38283</v>
@@ -5222,10 +4650,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>Malatya</t>
-        </is>
+      <c r="A46" s="1" t="n">
+        <v>44</v>
       </c>
       <c r="B46" t="n">
         <v>35351</v>
@@ -5238,10 +4664,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>Manisa</t>
-        </is>
+      <c r="A47" s="1" t="n">
+        <v>45</v>
       </c>
       <c r="B47" t="n">
         <v>84301</v>
@@ -5254,10 +4678,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>Kahramanmaraş</t>
-        </is>
+      <c r="A48" s="1" t="n">
+        <v>46</v>
       </c>
       <c r="B48" t="n">
         <v>40938</v>
@@ -5270,10 +4692,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>Mardin</t>
-        </is>
+      <c r="A49" s="1" t="n">
+        <v>47</v>
       </c>
       <c r="B49" t="n">
         <v>22341</v>
@@ -5286,10 +4706,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>Muğla</t>
-        </is>
+      <c r="A50" s="1" t="n">
+        <v>48</v>
       </c>
       <c r="B50" t="n">
         <v>50791</v>
@@ -5302,10 +4720,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>Muş</t>
-        </is>
+      <c r="A51" s="1" t="n">
+        <v>49</v>
       </c>
       <c r="B51" t="n">
         <v>10520</v>
@@ -5318,10 +4734,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>Nevşehir</t>
-        </is>
+      <c r="A52" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="B52" t="n">
         <v>17186</v>
@@ -5334,10 +4748,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>Niğde</t>
-        </is>
+      <c r="A53" s="1" t="n">
+        <v>51</v>
       </c>
       <c r="B53" t="n">
         <v>18454</v>
@@ -5350,10 +4762,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>Ordu</t>
-        </is>
+      <c r="A54" s="1" t="n">
+        <v>52</v>
       </c>
       <c r="B54" t="n">
         <v>50263</v>
@@ -5366,10 +4776,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>Rize</t>
-        </is>
+      <c r="A55" s="1" t="n">
+        <v>53</v>
       </c>
       <c r="B55" t="n">
         <v>23098</v>
@@ -5382,10 +4790,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>Sakarya</t>
-        </is>
+      <c r="A56" s="1" t="n">
+        <v>54</v>
       </c>
       <c r="B56" t="n">
         <v>54213</v>
@@ -5398,10 +4804,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>Samsun</t>
-        </is>
+      <c r="A57" s="1" t="n">
+        <v>55</v>
       </c>
       <c r="B57" t="n">
         <v>77345</v>
@@ -5414,10 +4818,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>Siirt</t>
-        </is>
+      <c r="A58" s="1" t="n">
+        <v>56</v>
       </c>
       <c r="B58" t="n">
         <v>8430</v>
@@ -5430,10 +4832,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>Sinop</t>
-        </is>
+      <c r="A59" s="1" t="n">
+        <v>57</v>
       </c>
       <c r="B59" t="n">
         <v>17714</v>
@@ -5446,10 +4846,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>Sivas</t>
-        </is>
+      <c r="A60" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="B60" t="n">
         <v>37476</v>
@@ -5462,10 +4860,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>Tekirdağ</t>
-        </is>
+      <c r="A61" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="B61" t="n">
         <v>51928</v>
@@ -5478,10 +4874,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>Tokat</t>
-        </is>
+      <c r="A62" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="B62" t="n">
         <v>40305</v>
@@ -5494,10 +4888,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>Trabzon</t>
-        </is>
+      <c r="A63" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="B63" t="n">
         <v>46249</v>
@@ -5510,10 +4902,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>Tunceli</t>
-        </is>
+      <c r="A64" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="B64" t="n">
         <v>5156</v>
@@ -5526,10 +4916,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>Şanlıurfa</t>
-        </is>
+      <c r="A65" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="B65" t="n">
         <v>45263</v>
@@ -5542,10 +4930,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>Uşak</t>
-        </is>
+      <c r="A66" s="1" t="n">
+        <v>64</v>
       </c>
       <c r="B66" t="n">
         <v>21154</v>
@@ -5558,10 +4944,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>Van</t>
-        </is>
+      <c r="A67" s="1" t="n">
+        <v>65</v>
       </c>
       <c r="B67" t="n">
         <v>28200</v>
@@ -5574,10 +4958,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>Yozgat</t>
-        </is>
+      <c r="A68" s="1" t="n">
+        <v>66</v>
       </c>
       <c r="B68" t="n">
         <v>25616</v>
@@ -5590,10 +4972,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>Zonguldak</t>
-        </is>
+      <c r="A69" s="1" t="n">
+        <v>67</v>
       </c>
       <c r="B69" t="n">
         <v>36853</v>
@@ -5606,10 +4986,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Aksaray</t>
-        </is>
+      <c r="A70" s="1" t="n">
+        <v>68</v>
       </c>
       <c r="B70" t="n">
         <v>18572</v>
@@ -5622,10 +5000,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>Bayburt</t>
-        </is>
+      <c r="A71" s="1" t="n">
+        <v>69</v>
       </c>
       <c r="B71" t="n">
         <v>4189</v>
@@ -5638,10 +5014,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>Karaman</t>
-        </is>
+      <c r="A72" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="B72" t="n">
         <v>12837</v>
@@ -5654,10 +5028,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>Kırıkkale</t>
-        </is>
+      <c r="A73" s="1" t="n">
+        <v>71</v>
       </c>
       <c r="B73" t="n">
         <v>16878</v>
@@ -5670,10 +5042,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Batman</t>
-        </is>
+      <c r="A74" s="1" t="n">
+        <v>72</v>
       </c>
       <c r="B74" t="n">
         <v>14696</v>
@@ -5686,10 +5056,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>Şırnak</t>
-        </is>
+      <c r="A75" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B75" t="n">
         <v>10347</v>
@@ -5702,10 +5070,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>Bartın</t>
-        </is>
+      <c r="A76" s="1" t="n">
+        <v>74</v>
       </c>
       <c r="B76" t="n">
         <v>13623</v>
@@ -5718,10 +5084,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Ardahan</t>
-        </is>
+      <c r="A77" s="1" t="n">
+        <v>75</v>
       </c>
       <c r="B77" t="n">
         <v>5723</v>
@@ -5734,10 +5098,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Iğdır</t>
-        </is>
+      <c r="A78" s="1" t="n">
+        <v>76</v>
       </c>
       <c r="B78" t="n">
         <v>7008</v>
@@ -5750,10 +5112,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>Yalova</t>
-        </is>
+      <c r="A79" s="1" t="n">
+        <v>77</v>
       </c>
       <c r="B79" t="n">
         <v>14960</v>
@@ -5766,10 +5126,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Karabük</t>
-        </is>
+      <c r="A80" s="1" t="n">
+        <v>78</v>
       </c>
       <c r="B80" t="n">
         <v>15524</v>
@@ -5782,10 +5140,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>Kilis</t>
-        </is>
+      <c r="A81" s="1" t="n">
+        <v>79</v>
       </c>
       <c r="B81" t="n">
         <v>6171</v>
@@ -5798,10 +5154,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Osmaniye</t>
-        </is>
+      <c r="A82" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="B82" t="n">
         <v>22599</v>
@@ -5814,10 +5168,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Düzce</t>
-        </is>
+      <c r="A83" s="1" t="n">
+        <v>81</v>
       </c>
       <c r="B83" t="n">
         <v>21414</v>

</xml_diff>